<commit_message>
update the script for creating setting env
update the script for creating setting env
</commit_message>
<xml_diff>
--- a/target/classes/Data/DataFile.xlsx
+++ b/target/classes/Data/DataFile.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_Login" sheetId="1" r:id="rId1"/>
     <sheet name="TC02_RegisterAccount" sheetId="2" r:id="rId2"/>
-    <sheet name="Resources" sheetId="3" r:id="rId3"/>
+    <sheet name="TC03_UpdatePassword" sheetId="4" r:id="rId3"/>
+    <sheet name="Resources" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="listcountry">Resources!$A$2:$A$3</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>UserName</t>
   </si>
@@ -53,16 +54,60 @@
   </si>
   <si>
     <t>List countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t>Country code</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t>Plate number</t>
+  </si>
+  <si>
+    <t>PT00000001</t>
+  </si>
+  <si>
+    <t>user317@gmail.com</t>
+  </si>
+  <si>
+    <t>491258667</t>
+  </si>
+  <si>
+    <t>Old password</t>
+  </si>
+  <si>
+    <t>New password</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>123456789aA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,16 +130,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,10 +457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,18 +477,106 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>listcountry</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>